<commit_message>
Updating comment analysis and gitignore
</commit_message>
<xml_diff>
--- a/Apps/YouTubeAnalysis/Analysis/Comments/CourseParticipation/Step03_GenerateYouTubeIdSubstring.xlsx
+++ b/Apps/YouTubeAnalysis/Analysis/Comments/CourseParticipation/Step03_GenerateYouTubeIdSubstring.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="153">
   <si>
     <t>Name</t>
   </si>
@@ -258,7 +258,7 @@
     <t>AE501_AB</t>
   </si>
   <si>
-    <t>AE501_CD</t>
+    <t>AE501_CB</t>
   </si>
   <si>
     <t>AE501_TB</t>
@@ -270,7 +270,7 @@
     <t>AE501_BB</t>
   </si>
   <si>
-    <t>AE501_KT</t>
+    <t>AE501_KC</t>
   </si>
   <si>
     <t>AE501_JC</t>
@@ -279,7 +279,7 @@
     <t>AE501_RC</t>
   </si>
   <si>
-    <t>AE501_UJ</t>
+    <t>AE501_UC</t>
   </si>
   <si>
     <t>AE501_LC</t>
@@ -321,9 +321,6 @@
     <t>AE501_DG</t>
   </si>
   <si>
-    <t>AE501_BN</t>
-  </si>
-  <si>
     <t>AE501_BH</t>
   </si>
   <si>
@@ -333,7 +330,7 @@
     <t>AE501_CJ</t>
   </si>
   <si>
-    <t>AE501_WH</t>
+    <t>AE501_WK</t>
   </si>
   <si>
     <t>AE501_EL</t>
@@ -378,7 +375,7 @@
     <t>AE501_KN</t>
   </si>
   <si>
-    <t>AE501_CR</t>
+    <t>AE501_CO</t>
   </si>
   <si>
     <t>AE501_YP</t>
@@ -396,13 +393,13 @@
     <t>AE501_GR</t>
   </si>
   <si>
-    <t>AE501_CR</t>
+    <t>AE501_CC</t>
   </si>
   <si>
     <t>AE501_BR</t>
   </si>
   <si>
-    <t>AE501_TS</t>
+    <t>AE501_TT</t>
   </si>
   <si>
     <t>AE501_MS</t>
@@ -432,7 +429,7 @@
     <t>AE501_DT</t>
   </si>
   <si>
-    <t>AE501_AG</t>
+    <t>AE501_AU</t>
   </si>
   <si>
     <t>AE501_AW</t>
@@ -451,6 +448,27 @@
   </si>
   <si>
     <t>Comment</t>
+  </si>
+  <si>
+    <t>Not a unique string ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last word in name appears to have some variation of Jr as a suffix.  </t>
+  </si>
+  <si>
+    <t>Not a unique string ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last word in name appears to have a /.  </t>
+  </si>
+  <si>
+    <t>Not a unique string ID</t>
+  </si>
+  <si>
+    <t>Last word in name appears to have a /.  Not a unique string ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last word in name appears to have a /.  </t>
   </si>
   <si>
     <t>Not a unique string ID</t>
@@ -505,7 +523,7 @@
     <col min="1" max="1" width="27.34765625" customWidth="true"/>
     <col min="2" max="2" width="10.89453125" customWidth="true"/>
     <col min="3" max="3" width="20.984375" customWidth="true"/>
-    <col min="4" max="4" width="19.2578125" customWidth="true"/>
+    <col min="4" max="4" width="57.2578125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -516,10 +534,10 @@
         <v>72</v>
       </c>
       <c r="C1" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="D1" s="0" t="s">
         <v>144</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="2">
@@ -734,9 +752,11 @@
         <v>90</v>
       </c>
       <c r="C19" s="0">
-        <v>0</v>
-      </c>
-      <c r="D19" s="0"/>
+        <v>1</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
@@ -782,9 +802,11 @@
         <v>94</v>
       </c>
       <c r="C23" s="0">
-        <v>0</v>
-      </c>
-      <c r="D23" s="0"/>
+        <v>1</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
@@ -878,28 +900,32 @@
         <v>102</v>
       </c>
       <c r="C31" s="0">
-        <v>0</v>
-      </c>
-      <c r="D31" s="0"/>
+        <v>1</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
         <v>31</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C32" s="0">
-        <v>0</v>
-      </c>
-      <c r="D32" s="0"/>
+        <v>1</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
         <v>32</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C33" s="0">
         <v>0</v>
@@ -911,7 +937,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C34" s="0">
         <v>0</v>
@@ -923,7 +949,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C35" s="0">
         <v>0</v>
@@ -935,7 +961,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C36" s="0">
         <v>0</v>
@@ -947,7 +973,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C37" s="0">
         <v>0</v>
@@ -959,7 +985,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C38" s="0">
         <v>0</v>
@@ -971,7 +997,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C39" s="0">
         <v>0</v>
@@ -983,13 +1009,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C40" s="0">
         <v>1</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="41">
@@ -997,25 +1023,27 @@
         <v>40</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C41" s="0">
-        <v>0</v>
-      </c>
-      <c r="D41" s="0"/>
+        <v>1</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="s">
         <v>41</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C42" s="0">
         <v>1</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="43">
@@ -1023,7 +1051,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C43" s="0">
         <v>0</v>
@@ -1035,7 +1063,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C44" s="0">
         <v>0</v>
@@ -1047,7 +1075,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C45" s="0">
         <v>0</v>
@@ -1059,7 +1087,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C46" s="0">
         <v>0</v>
@@ -1071,13 +1099,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C47" s="0">
         <v>1</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="48">
@@ -1085,7 +1113,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C48" s="0">
         <v>0</v>
@@ -1097,7 +1125,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C49" s="0">
         <v>0</v>
@@ -1109,21 +1137,19 @@
         <v>49</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C50" s="0">
-        <v>1</v>
-      </c>
-      <c r="D50" s="0" t="s">
-        <v>146</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D50" s="0"/>
     </row>
     <row r="51">
       <c r="A51" s="0" t="s">
         <v>50</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C51" s="0">
         <v>0</v>
@@ -1135,7 +1161,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C52" s="0">
         <v>0</v>
@@ -1147,7 +1173,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C53" s="0">
         <v>0</v>
@@ -1159,7 +1185,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C54" s="0">
         <v>0</v>
@@ -1171,7 +1197,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C55" s="0">
         <v>0</v>
@@ -1183,13 +1209,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C56" s="0">
         <v>1</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="57">
@@ -1197,7 +1223,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C57" s="0">
         <v>0</v>
@@ -1209,25 +1235,27 @@
         <v>57</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C58" s="0">
-        <v>0</v>
-      </c>
-      <c r="D58" s="0"/>
+        <v>1</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="s">
         <v>58</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C59" s="0">
         <v>1</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
     <row r="60">
@@ -1235,7 +1263,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C60" s="0">
         <v>0</v>
@@ -1247,13 +1275,13 @@
         <v>60</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C61" s="0">
         <v>1</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
     <row r="62">
@@ -1261,7 +1289,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C62" s="0">
         <v>0</v>
@@ -1273,7 +1301,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C63" s="0">
         <v>0</v>
@@ -1285,13 +1313,13 @@
         <v>63</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C64" s="0">
         <v>1</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
     <row r="65">
@@ -1299,7 +1327,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C65" s="0">
         <v>0</v>
@@ -1311,7 +1339,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C66" s="0">
         <v>0</v>
@@ -1323,7 +1351,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C67" s="0">
         <v>0</v>
@@ -1335,7 +1363,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C68" s="0">
         <v>0</v>
@@ -1347,13 +1375,13 @@
         <v>68</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C69" s="0">
         <v>1</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
     <row r="70">
@@ -1361,7 +1389,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C70" s="0">
         <v>0</v>
@@ -1373,13 +1401,13 @@
         <v>70</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C71" s="0">
         <v>1</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
     <row r="72">
@@ -1387,7 +1415,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C72" s="0">
         <v>0</v>

</xml_diff>